<commit_message>
update multi-link function list
</commit_message>
<xml_diff>
--- a/Multi-linkFunctionList.xlsx
+++ b/Multi-linkFunctionList.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25500" windowHeight="15120"/>
+    <workbookView windowWidth="25500" windowHeight="11330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,17 +14,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$5</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
   <si>
     <t>生产线</t>
   </si>
@@ -47,86 +42,7 @@
     <t>App生产线</t>
   </si>
   <si>
-    <t xml:space="preserve">add_library_XXX.pri
-add_include_LibName()
-add_library_LibName()
-add_defines_LibName()
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add_deploy()
-add_deploy_config()
-add_deploy_config_to()
-add_deploy_config_to_group()
-add_deploy_library()
-add_deploy_library_bundle()
-add_deploy_libraryes()
-has_deployed_library()
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add_include()
-add_include_bundle()
-add_library()
-add_library_bundle()
-add_link_library()
-add_link_library_bundle()
-add_library_path()
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">system_errcode()
-mkdir()
-empty_file()
-write_line()
-copy_dir_and_file()
-is_same_file()
-read_ini()
-write_ini()
-user_home()
-user_config_path()
-</t>
-  </si>
-  <si>
-    <t>Lib生产线</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add_sdk()
-add_sdk_to_Qt()
-add_sdk_header()
-clean_sdk()
-add_export()
-</t>
-  </si>
-  <si>
-    <t>备注</t>
-  </si>
-  <si>
-    <t>* 不要随便调用，内部有所调用，威力巨大，有度的。</t>
-  </si>
-  <si>
-    <t xml:space="preserve">这两层的函数，多数，参数1为libGroupName，参数2为libName，参数3为libRealName。参数3还经常省略。
-基本上没有更多的冗余参数，以避免用户在使用过程中迷糊。
-</t>
-  </si>
-  <si>
-    <t>还有相应的get函数</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add_library_XXX.pri
-这个文件App生产线实现、Lib生产线实现、Multi-link实现都可以。
-</t>
-  </si>
-  <si>
-    <t>关于删除add_link_manager()的决定
-它其实是专门为library而存在的管理器，管理library的链接依赖库的工作，而不会发布依赖库。
-在Multi-link里，我用add_dependent_manager()兼容了app使用依赖库的方式和lib使用链接库的方式。所以删除专门为lib准备的接口，使用app兼容lib接口。</t>
-  </si>
-  <si>
-    <t>多链接技术有点像可编程控制器PLC，应用于App和Lib生产线。用户自主选用一些函数装配生产线，对App、Lib的生产过程（从编译到产品）实现自动化管理。</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add_version()
+    <t>add_version()
 add_language()
 add_zh_CN()
 add_en_US()
@@ -157,15 +73,99 @@
 clean_target()
 add_include_path()
 add_create_dependent_manager()
+add_setting_deploy()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add_library_XXX.pri
+add_include_LibName()
+add_library_LibName()
+add_defines_LibName()
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">add_deploy()
+add_deploy_config()
+add_deploy_config_to()
+add_deploy_config_to_group()
+add_deploy_library()
+add_deploy_library_bundle()
+add_deploy_libraryes()
+has_deployed_library()
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add_include()
+add_include_bundle()
+add_library()
+add_library_bundle()
+add_link_library()
+add_link_library_bundle()
+add_library_path()
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">system_errcode()
+mkdir()
+empty_file()
+write_line()
+copy_dir_and_file()
+is_same_file()
+read_ini()
+write_ini()
+user_home()
+user_config_path()
+</t>
+  </si>
+  <si>
+    <t>Lib生产线</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add_sdk()
+add_sdk_to_Qt()
+add_sdk_header()
+clean_sdk()
+add_export()
+</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
+    <t>* 不要随便调用，内部有所调用，威力巨大，有度的。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">这两层的函数，多数，参数1为libGroupName，参数2为libName，参数3为libRealName。参数3还经常省略。
+基本上没有更多的冗余参数，以避免用户在使用过程中迷糊。
+</t>
+  </si>
+  <si>
+    <t>还有相应的get函数</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add_library_XXX.pri
+这个文件App生产线实现、Lib生产线实现、Multi-link实现都可以。
+</t>
+  </si>
+  <si>
+    <t>关于删除add_link_manager()的决定
+它其实是专门为library而存在的管理器，管理library的链接依赖库的工作，而不会发布依赖库。
+在Multi-link里，我用add_dependent_manager()兼容了app使用依赖库的方式和lib使用链接库的方式。所以删除专门为lib准备的接口，使用app兼容lib接口。</t>
+  </si>
+  <si>
+    <t>多链接技术有点像可编程控制器PLC，应用于App和Lib生产线。用户自主选用一些函数装配生产线，对App、Lib的生产过程（从编译到产品）实现自动化管理。</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,21 +174,345 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -196,13 +520,255 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -225,22 +791,60 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -531,34 +1135,34 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B3"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="39.3363636363636" customWidth="1"/>
     <col min="3" max="3" width="31.5" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="51.33203125" customWidth="1"/>
-    <col min="6" max="6" width="31.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="37.6636363636364" customWidth="1"/>
+    <col min="5" max="5" width="51.3363636363636" customWidth="1"/>
+    <col min="6" max="6" width="31.8363636363636" customWidth="1"/>
+    <col min="7" max="7" width="10.1636363636364" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" s="1" customFormat="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,148 +1182,139 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="153" customHeight="1">
+    <row r="2" ht="153" customHeight="1" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="9" t="s">
         <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="304" customHeight="1">
+    <row r="3" ht="304" customHeight="1" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="5"/>
       <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="10"/>
+        <v>13</v>
+      </c>
+      <c r="F3" s="5"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="48" customHeight="1">
+    <row r="4" ht="48" customHeight="1" spans="1:6">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="35" customHeight="1">
+    <row r="5" ht="35" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="51" customHeight="1">
+    <row r="6" ht="51" customHeight="1" spans="1:6">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="F2:F3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
   <printOptions gridLines="1"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>